<commit_message>
docs(production): gerber, BOM, position files for PCBWay
</commit_message>
<xml_diff>
--- a/to_PCBWay/bom/telemetry_box_01_BOM.xlsx
+++ b/to_PCBWay/bom/telemetry_box_01_BOM.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75d92559c3a49a38/database/Работа/Telerace/dev/telemetry_box_01/to_PCBWay/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75d92559c3a49a38/database/Работа/Telerace/dev/telemetry_box_dev/to_PCBWay/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="269" documentId="14_{E71BF769-2C3B-D64A-8155-B07206C45879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E596E5C-8E94-2B48-86D5-677DAA889CAB}"/>
+  <xr:revisionPtr revIDLastSave="277" documentId="14_{E71BF769-2C3B-D64A-8155-B07206C45879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D3036FF-4D0F-8440-A069-B9B04D8819C7}"/>
   <bookViews>
-    <workbookView xWindow="-4820" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="TransmitterL_v04_ST_ST" localSheetId="0">Лист1!$B$1:$K$28</definedName>
+    <definedName name="TransmitterL_v04_ST_ST" localSheetId="0">Лист1!$B$1:$K$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="148">
   <si>
     <t>CL03A104KA3NNNC</t>
   </si>
@@ -231,9 +231,6 @@
     <t xml:space="preserve">    R12</t>
   </si>
   <si>
-    <t xml:space="preserve">    S1</t>
-  </si>
-  <si>
     <t xml:space="preserve">    U1</t>
   </si>
   <si>
@@ -435,12 +432,6 @@
     <t>Thick Film Resistors - SMD 0 Ohms 50mW 0201 1%</t>
   </si>
   <si>
-    <t>RC0201FR-07510RL</t>
-  </si>
-  <si>
-    <t>Thick Film Resistors - SMD 510 Ohms 50 mW 0201 1%</t>
-  </si>
-  <si>
     <t>RC0201FR-072KL</t>
   </si>
   <si>
@@ -453,15 +444,6 @@
     <t>Thick Film Resistors - SMD 5.1 kOhms 50 mW 0201 1%</t>
   </si>
   <si>
-    <t>PTS526 SM08 SMTR2 LFS</t>
-  </si>
-  <si>
-    <t>Tactile Switches 50mA 12VDC, 5.2x5.2mm, 0.8mm H, 160gf, G leads, No ground pin, no actuator</t>
-  </si>
-  <si>
-    <t>C&amp;K Switches</t>
-  </si>
-  <si>
     <t>A9G</t>
   </si>
   <si>
@@ -492,15 +474,6 @@
     <t>1.2mm * 1mm</t>
   </si>
   <si>
-    <t>ASCKCR00-BU5V5020402</t>
-  </si>
-  <si>
-    <t>Standard LEDs - SMD 1608 Red</t>
-  </si>
-  <si>
-    <t>Broadcom Limited</t>
-  </si>
-  <si>
     <t>RF System on a Chip - SoC nRF52840-QIAA QFN 73L 7x7</t>
   </si>
   <si>
@@ -534,9 +507,6 @@
     <t xml:space="preserve">    C35, C36</t>
   </si>
   <si>
-    <t xml:space="preserve">    D1, D2, D3, D4</t>
-  </si>
-  <si>
     <t xml:space="preserve">    J2, J3</t>
   </si>
   <si>
@@ -546,13 +516,10 @@
     <t xml:space="preserve">    R2, R3</t>
   </si>
   <si>
-    <t xml:space="preserve">    R5, R10, R11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    R6, R7, R8, R9</t>
-  </si>
-  <si>
     <t xml:space="preserve">    R13, R14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    R10, R11</t>
   </si>
 </sst>
 </file>
@@ -889,15 +856,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="36.5" customWidth="1"/>
+    <col min="2" max="2" width="58.6640625" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
@@ -949,16 +916,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>18</v>
@@ -977,16 +944,16 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>18</v>
@@ -1005,16 +972,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>18</v>
@@ -1027,7 +994,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C5" s="1">
         <v>7</v>
@@ -1039,7 +1006,7 @@
         <v>29</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G5" s="1">
         <v>603</v>
@@ -1055,7 +1022,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C6" s="1">
         <v>12</v>
@@ -1092,10 +1059,10 @@
         <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="G7" s="1">
         <v>201</v>
@@ -1120,10 +1087,10 @@
         <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="G8" s="1">
         <v>201</v>
@@ -1139,7 +1106,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -1148,10 +1115,10 @@
         <v>22</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="G9" s="1">
         <v>201</v>
@@ -1167,7 +1134,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -1176,10 +1143,10 @@
         <v>22</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="G10" s="1">
         <v>201</v>
@@ -1195,7 +1162,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C11" s="1">
         <v>7</v>
@@ -1207,7 +1174,7 @@
         <v>32</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G11" s="1">
         <v>402</v>
@@ -1232,10 +1199,10 @@
         <v>22</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="G12" s="1">
         <v>201</v>
@@ -1260,10 +1227,10 @@
         <v>22</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="G13" s="1">
         <v>201</v>
@@ -1279,7 +1246,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C14" s="1">
         <v>4</v>
@@ -1288,10 +1255,10 @@
         <v>1</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="G14" s="1">
         <v>402</v>
@@ -1316,10 +1283,10 @@
         <v>22</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="G15" s="1">
         <v>402</v>
@@ -1344,10 +1311,10 @@
         <v>22</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="G16" s="1">
         <v>402</v>
@@ -1372,10 +1339,10 @@
         <v>22</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="G17" s="1">
         <v>402</v>
@@ -1400,10 +1367,10 @@
         <v>22</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="G18" s="1">
         <v>402</v>
@@ -1419,19 +1386,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1452,10 +1419,10 @@
         <v>22</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="G20" s="1">
         <v>402</v>
@@ -1480,10 +1447,10 @@
         <v>22</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="G21" s="1">
         <v>201</v>
@@ -1496,50 +1463,46 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>152</v>
+        <v>41</v>
       </c>
       <c r="C22" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>138</v>
+        <v>93</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G22" s="1">
-        <v>603</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>41</v>
+        <v>143</v>
       </c>
       <c r="C23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1548,22 +1511,22 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>153</v>
+        <v>42</v>
       </c>
       <c r="C24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1572,34 +1535,38 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>100</v>
+        <v>22</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+        <v>103</v>
+      </c>
+      <c r="G25" s="1">
+        <v>805</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -1608,13 +1575,13 @@
         <v>22</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G26" s="1">
-        <v>805</v>
+        <v>402</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>18</v>
@@ -1624,25 +1591,25 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>44</v>
+        <v>144</v>
       </c>
       <c r="C27" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G27" s="1">
-        <v>402</v>
+        <v>603</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>18</v>
@@ -1652,25 +1619,25 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>154</v>
+        <v>45</v>
       </c>
       <c r="C28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G28" s="1">
-        <v>603</v>
+        <v>402</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>18</v>
@@ -1680,10 +1647,10 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
@@ -1692,10 +1659,10 @@
         <v>22</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G29" s="1">
         <v>402</v>
@@ -1708,10 +1675,10 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
@@ -1720,10 +1687,10 @@
         <v>22</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G30" s="1">
         <v>402</v>
@@ -1736,25 +1703,25 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G31" s="1">
-        <v>402</v>
+        <v>201</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>18</v>
@@ -1764,22 +1731,22 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>48</v>
+        <v>145</v>
       </c>
       <c r="C32" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>115</v>
+        <v>16</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>116</v>
+        <v>17</v>
       </c>
       <c r="G32" s="1">
         <v>201</v>
@@ -1792,22 +1759,22 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>155</v>
+        <v>49</v>
       </c>
       <c r="C33" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="G33" s="1">
         <v>201</v>
@@ -1820,22 +1787,22 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>49</v>
+        <v>147</v>
       </c>
       <c r="C34" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>117</v>
+        <v>19</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>118</v>
+        <v>20</v>
       </c>
       <c r="G34" s="1">
         <v>201</v>
@@ -1848,22 +1815,22 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>156</v>
+        <v>50</v>
       </c>
       <c r="C35" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="G35" s="1">
         <v>201</v>
@@ -1876,22 +1843,22 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C36" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G36" s="1">
         <v>201</v>
@@ -1904,78 +1871,70 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G37" s="1">
-        <v>201</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>158</v>
+        <v>52</v>
       </c>
       <c r="C38" s="1">
-        <v>2</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G38" s="1">
-        <v>201</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C39" s="1">
         <v>1</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>127</v>
+        <v>5</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -1984,163 +1943,100 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C40" s="1">
         <v>1</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>144</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C41" s="1">
         <v>1</v>
       </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1" t="s">
+      <c r="D41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G41" s="1"/>
+      <c r="G41" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C42" s="1">
         <v>1</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>129</v>
+        <v>4</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G42" s="1"/>
+      <c r="G42" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" s="1">
-        <v>1</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C44" s="1">
-        <v>1</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
+      <c r="A44" s="1"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" s="1">
-        <v>1</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
+      <c r="A45" s="1"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
@@ -2222,15 +2118,6 @@
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix(production): gerber, BOM, position files for PCBWay -successful production of modules
</commit_message>
<xml_diff>
--- a/to_PCBWay/bom/telemetry_box_01_BOM.xlsx
+++ b/to_PCBWay/bom/telemetry_box_01_BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75d92559c3a49a38/database/Работа/Telerace/dev/telemetry_box_dev/to_PCBWay/bom/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75d92559c3a49a38/database/Работа/Telerace/dev/telemetry_box_dev/to_PCBWay/bom/fix0423/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="349" documentId="14_{E71BF769-2C3B-D64A-8155-B07206C45879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A555FC23-FAA5-AE4A-9D58-5997E617AC74}"/>
+  <xr:revisionPtr revIDLastSave="360" documentId="14_{E71BF769-2C3B-D64A-8155-B07206C45879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24A50C40-B8BB-0F4D-B509-772000BF15AF}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="TransmitterL_v04_ST_ST" localSheetId="0">Лист1!$B$1:$K$22</definedName>
+    <definedName name="TransmitterL_v04_ST_ST" localSheetId="0">Лист1!$B$1:$K$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="138">
   <si>
     <t>CL03A104KA3NNNC</t>
   </si>
@@ -174,12 +174,6 @@
     <t xml:space="preserve">    C32</t>
   </si>
   <si>
-    <t xml:space="preserve">    C33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    C34</t>
-  </si>
-  <si>
     <t xml:space="preserve">    C39</t>
   </si>
   <si>
@@ -201,9 +195,6 @@
     <t xml:space="preserve">    L6</t>
   </si>
   <si>
-    <t xml:space="preserve">    L7</t>
-  </si>
-  <si>
     <t xml:space="preserve">    R1</t>
   </si>
   <si>
@@ -288,18 +279,6 @@
     <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 1uF+/-10% 16V X5R 10 0402</t>
   </si>
   <si>
-    <t>GJM1555C1HR80DB01J</t>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0.8 pF 50 VDC 0.5 pF 0402 C0G (NP0)</t>
-  </si>
-  <si>
-    <t>GJM1555C1H2R7BB01D</t>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 2.7 pF 50 VDC 0.1 pF 0402 C0G (NP0)</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -355,12 +334,6 @@
   </si>
   <si>
     <t>RF Inductors - SMD 12 NH 5%</t>
-  </si>
-  <si>
-    <t>LQW15AN3N6B8ZD</t>
-  </si>
-  <si>
-    <t>RF Inductors - SMD 3.6 NH +-.1NH</t>
   </si>
   <si>
     <t>RC0201FR-07200KL</t>
@@ -860,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="B40" sqref="B40:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -920,16 +893,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>18</v>
@@ -942,7 +915,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C3" s="1">
         <v>7</v>
@@ -954,7 +927,7 @@
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G3" s="1">
         <v>603</v>
@@ -970,7 +943,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C4" s="1">
         <v>13</v>
@@ -1007,10 +980,10 @@
         <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G5" s="1">
         <v>201</v>
@@ -1035,10 +1008,10 @@
         <v>22</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G6" s="1">
         <v>201</v>
@@ -1054,7 +1027,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -1063,10 +1036,10 @@
         <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G7" s="1">
         <v>201</v>
@@ -1082,7 +1055,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -1091,10 +1064,10 @@
         <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G8" s="1">
         <v>201</v>
@@ -1110,7 +1083,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C9" s="1">
         <v>7</v>
@@ -1122,7 +1095,7 @@
         <v>28</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G9" s="1">
         <v>402</v>
@@ -1147,10 +1120,10 @@
         <v>22</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G10" s="1">
         <v>201</v>
@@ -1175,10 +1148,10 @@
         <v>22</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="G11" s="1">
         <v>201</v>
@@ -1203,10 +1176,10 @@
         <v>22</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G12" s="1">
         <v>201</v>
@@ -1222,7 +1195,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C13" s="1">
         <v>4</v>
@@ -1231,10 +1204,10 @@
         <v>1</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G13" s="1">
         <v>402</v>
@@ -1250,26 +1223,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="1">
-        <v>402</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
@@ -1278,7 +1247,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -1287,10 +1256,10 @@
         <v>22</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G15" s="1">
         <v>402</v>
@@ -1306,19 +1275,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>129</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1336,20 +1305,16 @@
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="1">
-        <v>402</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
@@ -1364,16 +1329,20 @@
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>78</v>
+        <v>22</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="G18" s="1">
+        <v>805</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
@@ -1388,16 +1357,20 @@
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>80</v>
+        <v>22</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="G19" s="1">
+        <v>402</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
@@ -1406,22 +1379,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="C20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G20" s="1">
-        <v>805</v>
+        <v>603</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>18</v>
@@ -1434,7 +1407,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -1443,10 +1416,10 @@
         <v>22</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G21" s="1">
         <v>402</v>
@@ -1462,22 +1435,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>122</v>
+        <v>38</v>
       </c>
       <c r="C22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G22" s="1">
-        <v>603</v>
+        <v>402</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>18</v>
@@ -1496,16 +1469,16 @@
         <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G23" s="1">
-        <v>402</v>
+        <v>201</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>18</v>
@@ -1518,22 +1491,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="C24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="G24" s="1">
-        <v>402</v>
+        <v>201</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>18</v>
@@ -1546,22 +1519,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G25" s="1">
-        <v>402</v>
+        <v>201</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>18</v>
@@ -1574,19 +1547,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="C26" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>95</v>
+        <v>19</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="G26" s="1">
         <v>201</v>
@@ -1602,19 +1575,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>123</v>
+        <v>41</v>
       </c>
       <c r="C27" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="G27" s="1">
         <v>201</v>
@@ -1630,19 +1603,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>43</v>
+        <v>115</v>
       </c>
       <c r="C28" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G28" s="1">
         <v>201</v>
@@ -1658,25 +1631,23 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="C29" s="1">
-        <v>2</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="1">
-        <v>201</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -1686,26 +1657,24 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>15</v>
+        <v>105</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G30" s="1">
-        <v>201</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
@@ -1714,26 +1683,20 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>124</v>
+        <v>43</v>
       </c>
       <c r="C31" s="1">
-        <v>2</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G31" s="1">
-        <v>201</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
@@ -1742,24 +1705,22 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>130</v>
+        <v>44</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>131</v>
+        <v>5</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>133</v>
+        <v>96</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
@@ -1774,17 +1735,15 @@
         <v>1</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>116</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -1793,21 +1752,25 @@
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>46</v>
+      <c r="B34" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
       </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>103</v>
+      <c r="D34" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="H34" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
@@ -1815,23 +1778,25 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>47</v>
+      <c r="B35" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="C35" s="1">
         <v>1</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>5</v>
+        <v>131</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
+      <c r="H35" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
@@ -1839,23 +1804,27 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>48</v>
+      <c r="B36" s="4" t="s">
+        <v>128</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
+        <v>135</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
@@ -1863,25 +1832,25 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>135</v>
+      <c r="B37" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>141</v>
+        <v>2</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
@@ -1889,119 +1858,48 @@
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>136</v>
+      <c r="B38" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C38" s="1">
         <v>1</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>140</v>
+        <v>3</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>138</v>
+        <v>4</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C39" s="1">
-        <v>1</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="1">
-        <v>1</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
+      <c r="A40" s="1"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C41" s="1">
-        <v>1</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
+      <c r="A41" s="1"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
@@ -2083,15 +1981,6 @@
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>